<commit_message>
Adding RunTotalAnalysisLotun function to FEModel
</commit_message>
<xml_diff>
--- a/testLotung/LotungProperties2.xlsx
+++ b/testLotung/LotungProperties2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PArduino\Documents\research\GiTHub\SiteResponseTool-1\testLotung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parduino\Documents\Research\GitHub\SiteResponseTool-1\testLotung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23595" windowHeight="10605" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23595" windowHeight="10605"/>
   </bookViews>
   <sheets>
     <sheet name="Profile" sheetId="5" r:id="rId1"/>
@@ -1102,32 +1102,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB49"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.73046875" customWidth="1"/>
-    <col min="4" max="4" width="12.73046875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.73046875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="13.59765625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="13" max="13" width="12.1328125" customWidth="1"/>
-    <col min="14" max="14" width="14.1328125" customWidth="1"/>
-    <col min="15" max="15" width="17.1328125" customWidth="1"/>
-    <col min="16" max="16" width="8.265625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.265625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.3984375" style="1" customWidth="1"/>
-    <col min="19" max="20" width="11.59765625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="17.1328125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1328125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="12.73046875" customWidth="1"/>
-    <col min="28" max="28" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" style="1" customWidth="1"/>
+    <col min="19" max="20" width="11.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="17.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" customWidth="1"/>
+    <col min="28" max="28" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>0+1</f>
         <v>1</v>
@@ -1261,16 +1261,16 @@
       <c r="Y3" s="6">
         <v>0</v>
       </c>
-      <c r="Z3" s="3">
-        <f>2*1/(2*PI()*0.65)</f>
-        <v>0.48970751720583183</v>
+      <c r="Z3" s="9">
+        <f>2*1/(2*PI()*0.65)/100</f>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB3">
         <f>U3*(T3*T3-4/3*S3*S3)</f>
         <v>616666666.66666615</v>
       </c>
     </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <f t="shared" ref="B4:B23" si="4">B3+1</f>
         <v>2</v>
@@ -1345,16 +1345,16 @@
       <c r="Y4" s="6">
         <v>0</v>
       </c>
-      <c r="Z4" s="3">
-        <f t="shared" ref="Z4:Z24" si="9">2*1/(2*PI()*0.65)</f>
-        <v>0.48970751720583183</v>
+      <c r="Z4" s="9">
+        <f t="shared" ref="Z4:Z24" si="9">2*1/(2*PI()*0.65)/100</f>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB4" s="1">
         <f t="shared" ref="AB4:AB24" si="10">U4*(T4*T4-4/3*S4*S4)</f>
         <v>716874999.99999952</v>
       </c>
     </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <f t="shared" si="4"/>
         <v>3</v>
@@ -1430,16 +1430,16 @@
       <c r="Y5" s="6">
         <v>0</v>
       </c>
-      <c r="Z5" s="3">
+      <c r="Z5" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB5" s="1">
         <f t="shared" si="10"/>
         <v>817083333.33333254</v>
       </c>
     </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -1514,16 +1514,16 @@
       <c r="Y6" s="6">
         <v>0</v>
       </c>
-      <c r="Z6" s="3">
+      <c r="Z6" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB6" s="1">
         <f t="shared" si="10"/>
         <v>917291666.66666591</v>
       </c>
     </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -1598,16 +1598,16 @@
       <c r="Y7" s="6">
         <v>0</v>
       </c>
-      <c r="Z7" s="3">
+      <c r="Z7" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB7" s="1">
         <f t="shared" si="10"/>
         <v>1017499999.9999989</v>
       </c>
     </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -1682,16 +1682,16 @@
       <c r="Y8" s="6">
         <v>0</v>
       </c>
-      <c r="Z8" s="3">
+      <c r="Z8" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB8" s="1">
         <f t="shared" si="10"/>
         <v>1117708333.3333325</v>
       </c>
     </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -1766,16 +1766,16 @@
       <c r="Y9" s="6">
         <v>0</v>
       </c>
-      <c r="Z9" s="3">
+      <c r="Z9" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB9" s="1">
         <f t="shared" si="10"/>
         <v>1217916666.6666656</v>
       </c>
     </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <f t="shared" si="4"/>
         <v>8</v>
@@ -1850,16 +1850,16 @@
       <c r="Y10" s="6">
         <v>0</v>
       </c>
-      <c r="Z10" s="3">
+      <c r="Z10" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB10" s="1">
         <f t="shared" si="10"/>
         <v>1318124999.9999988</v>
       </c>
     </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -1934,16 +1934,16 @@
       <c r="Y11" s="6">
         <v>0</v>
       </c>
-      <c r="Z11" s="3">
+      <c r="Z11" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB11" s="1">
         <f t="shared" si="10"/>
         <v>1418333333.3333318</v>
       </c>
     </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2018,16 +2018,16 @@
       <c r="Y12" s="6">
         <v>0</v>
       </c>
-      <c r="Z12" s="3">
+      <c r="Z12" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB12" s="1">
         <f t="shared" si="10"/>
         <v>1518541666.6666653</v>
       </c>
     </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2102,16 +2102,16 @@
       <c r="Y13" s="6">
         <v>0</v>
       </c>
-      <c r="Z13" s="3">
+      <c r="Z13" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB13" s="1">
         <f t="shared" si="10"/>
         <v>1618749999.9999986</v>
       </c>
     </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2180,16 +2180,16 @@
       <c r="Y14" s="6">
         <v>0</v>
       </c>
-      <c r="Z14" s="3">
+      <c r="Z14" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB14" s="1">
         <f t="shared" si="10"/>
         <v>1718958333.3333318</v>
       </c>
     </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2258,16 +2258,16 @@
       <c r="Y15" s="6">
         <v>0</v>
       </c>
-      <c r="Z15" s="3">
+      <c r="Z15" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB15" s="1">
         <f t="shared" si="10"/>
         <v>1819166666.6666648</v>
       </c>
     </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2336,16 +2336,16 @@
       <c r="Y16" s="6">
         <v>0</v>
       </c>
-      <c r="Z16" s="3">
+      <c r="Z16" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB16" s="1">
         <f t="shared" si="10"/>
         <v>1919374999.9999988</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2414,16 +2414,16 @@
       <c r="Y17" s="6">
         <v>0</v>
       </c>
-      <c r="Z17" s="3">
+      <c r="Z17" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB17" s="1">
         <f t="shared" si="10"/>
         <v>2019583333.3333318</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -2492,16 +2492,16 @@
       <c r="Y18" s="6">
         <v>0</v>
       </c>
-      <c r="Z18" s="3">
+      <c r="Z18" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB18" s="1">
         <f t="shared" si="10"/>
         <v>2119791666.6666651</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
@@ -2570,16 +2570,16 @@
       <c r="Y19" s="6">
         <v>0</v>
       </c>
-      <c r="Z19" s="3">
+      <c r="Z19" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB19" s="1">
         <f t="shared" si="10"/>
         <v>2219999999.9999986</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -2646,16 +2646,16 @@
       <c r="Y20" s="6">
         <v>0</v>
       </c>
-      <c r="Z20" s="3">
+      <c r="Z20" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB20" s="1">
         <f t="shared" si="10"/>
         <v>2836666666.6666641</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <f t="shared" si="4"/>
         <v>19</v>
@@ -2722,16 +2722,16 @@
       <c r="Y21" s="6">
         <v>0</v>
       </c>
-      <c r="Z21" s="3">
+      <c r="Z21" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB21" s="1">
         <f t="shared" si="10"/>
         <v>2466666666.6666651</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -2798,16 +2798,16 @@
       <c r="Y22" s="6">
         <v>0</v>
       </c>
-      <c r="Z22" s="3">
+      <c r="Z22" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB22" s="1">
         <f t="shared" si="10"/>
         <v>4439999999.9999952</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <f t="shared" si="4"/>
         <v>21</v>
@@ -2874,16 +2874,16 @@
       <c r="Y23" s="6">
         <v>0</v>
       </c>
-      <c r="Z23" s="3">
+      <c r="Z23" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB23" s="1">
         <f t="shared" si="10"/>
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>5</v>
       </c>
@@ -2942,16 +2942,16 @@
       <c r="Y24" s="6">
         <v>0</v>
       </c>
-      <c r="Z24" s="3">
+      <c r="Z24" s="9">
         <f t="shared" si="9"/>
-        <v>0.48970751720583183</v>
+        <v>4.897075172058318E-3</v>
       </c>
       <c r="AB24" s="1">
         <f t="shared" si="10"/>
         <v>7399999999.9999924</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="4" t="s">
         <v>0</v>
@@ -2970,7 +2970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1">
         <f>0+1</f>
@@ -2993,7 +2993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1">
         <f t="shared" ref="B29:B48" si="15">B28+1</f>
@@ -3016,7 +3016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1">
         <f t="shared" si="15"/>
@@ -3039,7 +3039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1">
         <f t="shared" si="15"/>
@@ -3062,7 +3062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1">
         <f t="shared" si="15"/>
@@ -3085,7 +3085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1">
         <f t="shared" si="15"/>
@@ -3108,7 +3108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1">
         <f t="shared" si="15"/>
@@ -3131,7 +3131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1">
         <f t="shared" si="15"/>
@@ -3154,7 +3154,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1">
         <f t="shared" si="15"/>
@@ -3177,7 +3177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1">
         <f t="shared" si="15"/>
@@ -3200,7 +3200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1">
         <f t="shared" si="15"/>
@@ -3223,7 +3223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1">
         <f t="shared" si="15"/>
@@ -3246,7 +3246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1">
         <f t="shared" si="15"/>
@@ -3269,7 +3269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1">
         <f t="shared" si="15"/>
@@ -3292,7 +3292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1">
         <f t="shared" si="15"/>
@@ -3315,7 +3315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1">
         <f t="shared" si="15"/>
@@ -3338,7 +3338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1">
         <f t="shared" si="15"/>
@@ -3361,7 +3361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1">
         <f t="shared" si="15"/>
@@ -3384,7 +3384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1">
         <f t="shared" si="15"/>
@@ -3407,7 +3407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1">
         <f t="shared" si="15"/>
@@ -3430,7 +3430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1">
         <f t="shared" si="15"/>
@@ -3453,7 +3453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
         <v>5</v>
@@ -3481,20 +3481,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="1"/>
-    <col min="2" max="11" width="12.73046875" style="1" customWidth="1"/>
-    <col min="12" max="14" width="9.1328125" style="1"/>
-    <col min="15" max="15" width="11.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="11" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>39</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>616666666.66666615</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>716874999.99999952</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>817083333.33333254</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>917291666.66666591</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>1017499999.9999989</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>1117708333.3333325</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>41</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>1217916666.6666656</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>42</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>1318124999.9999988</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>1418333333.3333318</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>1518541666.6666653</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>1618749999.9999986</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>46</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>1718958333.3333318</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>47</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>1819166666.6666648</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>48</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>1919374999.9999988</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>49</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>2019583333.3333318</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>2119791666.6666651</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>51</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>2219999999.9999986</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -4276,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>52</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>2836666666.6666641</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>2836666666.6666641</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>54</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>2836666666.6666641</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>55</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>2836666666.6666641</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>56</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>2836666666.6666641</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>57</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>2836666666.6666641</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -4553,7 +4553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>58</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>2466666666.6666651</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>59</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>2466666666.6666651</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>60</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>2466666666.6666651</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>61</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>2466666666.6666651</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>62</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>2466666666.6666651</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>63</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>2466666666.6666651</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -4830,7 +4830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>64</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>4439999999.9999952</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>65</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>4439999999.9999952</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>66</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>4439999999.9999952</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>67</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>4439999999.9999952</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>68</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>4439999999.9999952</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>69</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>4439999999.9999952</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -5107,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>70</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>71</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>72</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>73</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>74</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>75</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>76</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>77</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>78</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>79</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>80</v>
       </c>
@@ -5580,7 +5580,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>81</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>3206666666.6666636</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -5642,7 +5642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>5</v>
       </c>
@@ -5699,15 +5699,15 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1328125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>25</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>2066.1157024793388</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>90</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>1946.998377501352</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>115</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>115</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>1736.1111111111111</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>1736.1111111111111</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>180</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>1873.0489073881374</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>180</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>1873.0489073881374</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>130</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>1851.192595229619</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>130</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>1851.192595229619</v>
       </c>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H26">
         <v>26.9</v>
       </c>
@@ -5844,9 +5844,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>110</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>215</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>250</v>
       </c>
@@ -5870,7 +5870,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>250</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>240</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>240</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>-29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>310</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>-29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>310</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>-35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>265</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>-35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>265</v>
       </c>
@@ -5939,12 +5939,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.73046875" style="2"/>
+    <col min="1" max="1" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <f>'G0Profile(MPa)_Borja2000'!A1*1000000/'VsProfile(ms)_Borja1999'!A1^2</f>
         <v>2066.1157024793388</v>
@@ -5953,7 +5953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>'G0Profile(MPa)_Borja2000'!A2*1000000/'VsProfile(ms)_Borja1999'!A2^2</f>
         <v>1946.998377501352</v>
@@ -5962,7 +5962,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>'G0Profile(MPa)_Borja2000'!A3*1000000/'VsProfile(ms)_Borja1999'!A3^2</f>
         <v>1840</v>
@@ -5971,7 +5971,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>'G0Profile(MPa)_Borja2000'!A4*1000000/'VsProfile(ms)_Borja1999'!A4^2</f>
         <v>1840</v>
@@ -5980,7 +5980,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>'G0Profile(MPa)_Borja2000'!A5*1000000/'VsProfile(ms)_Borja1999'!A5^2</f>
         <v>1736.1111111111111</v>
@@ -5989,7 +5989,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>'G0Profile(MPa)_Borja2000'!A6*1000000/'VsProfile(ms)_Borja1999'!A6^2</f>
         <v>1736.1111111111111</v>
@@ -5998,7 +5998,7 @@
         <v>-29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>'G0Profile(MPa)_Borja2000'!A7*1000000/'VsProfile(ms)_Borja1999'!A7^2</f>
         <v>1873.0489073881374</v>
@@ -6007,7 +6007,7 @@
         <v>-29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>'G0Profile(MPa)_Borja2000'!A8*1000000/'VsProfile(ms)_Borja1999'!A8^2</f>
         <v>1873.0489073881374</v>
@@ -6016,7 +6016,7 @@
         <v>-35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>'G0Profile(MPa)_Borja2000'!A9*1000000/'VsProfile(ms)_Borja1999'!A9^2</f>
         <v>1851.192595229619</v>
@@ -6025,7 +6025,7 @@
         <v>-35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>'G0Profile(MPa)_Borja2000'!A10*1000000/'VsProfile(ms)_Borja1999'!A10^2</f>
         <v>1851.192595229619</v>
@@ -6048,9 +6048,9 @@
       <selection sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0.48</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.48</v>
       </c>
@@ -6066,7 +6066,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.48</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.48</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.48</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.48</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>-29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.48</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>-29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.48</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>-35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.48</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>-35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.48</v>
       </c>

</xml_diff>